<commit_message>
Test fixes: buffers must have unique item-location
</commit_message>
<xml_diff>
--- a/doc/cookbook/operation/operation-posttime.xlsx
+++ b/doc/cookbook/operation/operation-posttime.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\develop\frepple.community\doc\cookbook\operation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="263" yWindow="1943" windowWidth="22718" windowHeight="5895" tabRatio="768" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16493" windowHeight="7545" tabRatio="768"/>
   </bookViews>
   <sheets>
     <sheet name="buffer" sheetId="1" r:id="rId1"/>
@@ -26,6 +21,7 @@
     <sheet name="parameter" sheetId="19" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <oleSize ref="A1:L24"/>
 </workbook>
 </file>
 
@@ -19814,8 +19810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -19874,8 +19870,8 @@
       <c r="C3" t="s">
         <v>6463</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
+      <c r="D3" s="2" t="s">
+        <v>6474</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -69008,7 +69004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -69239,7 +69235,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>